<commit_message>
added first horror event H5
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5CE638-5696-4490-9606-062A3A528179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1451EE-C72A-4A72-B9AC-C41A4597DC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="124">
   <si>
     <t>Quests</t>
   </si>
@@ -397,6 +397,15 @@
   </si>
   <si>
     <t>randomly: glowing eyes in the room, disappearing when turning on the lights again</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>%DoneSat</t>
+  </si>
+  <si>
+    <t>(fine-tuning)</t>
   </si>
 </sst>
 </file>
@@ -434,9 +443,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -446,10 +464,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -732,68 +762,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S26"/>
+  <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="Q2" s="1" t="s">
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="2"/>
+      <c r="S2" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V2" s="2"/>
+    </row>
+    <row r="3" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -805,66 +846,78 @@
       <c r="J3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="S3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="U3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
       <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" t="s">
         <v>92</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="5" t="s">
         <v>46</v>
       </c>
       <c r="H4" t="s">
         <v>24</v>
       </c>
       <c r="I4" t="str">
-        <f>L7</f>
+        <f>M7</f>
         <v>H4</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>98</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
       <c r="B5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" t="s">
         <v>93</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5" t="s">
         <v>47</v>
       </c>
       <c r="H5" t="s">
@@ -873,68 +926,68 @@
       <c r="J5" t="s">
         <v>103</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>5</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
       <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" t="s">
         <v>94</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>48</v>
       </c>
       <c r="H6" t="s">
         <v>25</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE(G5,", ",Q4)</f>
+        <f>CONCATENATE(G5,", ",S4)</f>
         <v>T2, O1</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>7</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
       <c r="B7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" t="s">
         <v>95</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="5" t="s">
         <v>49</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H8" t="s">
@@ -944,18 +997,24 @@
         <f>G7</f>
         <v>T4</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="Q8" s="6">
+        <v>0.92</v>
+      </c>
+      <c r="R8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>74</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H9" t="s">
@@ -965,118 +1024,118 @@
         <f>G8</f>
         <v>T5</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>14</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>75</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H10" t="s">
         <v>100</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>22</v>
       </c>
-      <c r="N10" t="str">
-        <f>L9</f>
+      <c r="O10" t="str">
+        <f>M9</f>
         <v>H6</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>76</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="5" t="s">
         <v>53</v>
       </c>
       <c r="H11" t="s">
         <v>101</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>77</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="5" t="s">
         <v>54</v>
       </c>
       <c r="H12" t="s">
         <v>110</v>
       </c>
       <c r="I12" t="str">
-        <f>L17</f>
+        <f>M17</f>
         <v>H14</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>78</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="5" t="s">
         <v>55</v>
       </c>
       <c r="H13" t="s">
         <v>112</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>105</v>
       </c>
-      <c r="N13" t="str">
+      <c r="O13" t="str">
         <f>G6</f>
         <v>T3</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>79</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="5" t="s">
         <v>56</v>
       </c>
       <c r="H14" t="s">
         <v>113</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>80</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="5" t="s">
         <v>57</v>
       </c>
       <c r="H15" t="s">
@@ -1088,169 +1147,179 @@
       <c r="J15" t="s">
         <v>117</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>81</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>82</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>83</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>111</v>
       </c>
-      <c r="N18" t="str">
+      <c r="O18" t="str">
         <f>G12</f>
         <v>T9</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>84</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>85</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>86</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>87</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>119</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>88</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>89</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>90</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>91</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" s="5" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="M2:P2"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="Q1:Q1048576 V1:V1048576 K1:K1048576 E1:E1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added horror event H4 (with more lamps, light switches, fuse box); bug fixes; added and fixed footsteps for meta player
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1451EE-C72A-4A72-B9AC-C41A4597DC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54267CD5-4741-4C17-818A-ABB8E58BC1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="126">
   <si>
     <t>Quests</t>
   </si>
@@ -405,7 +405,13 @@
     <t>%DoneSat</t>
   </si>
   <si>
-    <t>(fine-tuning)</t>
+    <t>(silent creepy noise, footsteps, combination with light?)</t>
+  </si>
+  <si>
+    <t>fusebox accessable</t>
+  </si>
+  <si>
+    <t>(MainSound(On/Off), FuseSound, metallic Box Sound, torchlight?)</t>
   </si>
 </sst>
 </file>
@@ -470,9 +476,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -480,6 +483,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -765,7 +771,7 @@
   <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,45 +781,45 @@
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="46.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="60.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="2"/>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
       <c r="K2" s="2"/>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
       <c r="Q2" s="2"/>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>96</v>
       </c>
       <c r="V2" s="2"/>
@@ -834,7 +840,7 @@
       <c r="E3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -849,7 +855,7 @@
       <c r="K3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -864,7 +870,7 @@
       <c r="Q3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="T3" s="1" t="s">
@@ -884,7 +890,7 @@
       <c r="B4" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>46</v>
       </c>
       <c r="H4" t="s">
@@ -894,13 +900,13 @@
         <f>M7</f>
         <v>H4</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="N4" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="4" t="s">
         <v>97</v>
       </c>
       <c r="T4" t="s">
@@ -917,7 +923,7 @@
       <c r="B5" t="s">
         <v>93</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>47</v>
       </c>
       <c r="H5" t="s">
@@ -926,7 +932,7 @@
       <c r="J5" t="s">
         <v>103</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="N5" t="s">
@@ -943,7 +949,7 @@
       <c r="B6" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H6" t="s">
@@ -953,7 +959,7 @@
         <f>CONCATENATE(G5,", ",S4)</f>
         <v>T2, O1</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="N6" t="s">
@@ -970,24 +976,33 @@
       <c r="B7" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>49</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="N7" t="s">
         <v>8</v>
+      </c>
+      <c r="P7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="R7" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="H8" t="s">
@@ -997,14 +1012,14 @@
         <f>G7</f>
         <v>T4</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="N8" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="6">
-        <v>0.92</v>
+      <c r="Q8" s="5">
+        <v>0.85</v>
       </c>
       <c r="R8" t="s">
         <v>123</v>
@@ -1014,7 +1029,7 @@
       <c r="A9" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>51</v>
       </c>
       <c r="H9" t="s">
@@ -1024,7 +1039,7 @@
         <f>G8</f>
         <v>T5</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="N9" t="s">
@@ -1038,13 +1053,13 @@
       <c r="A10" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H10" t="s">
         <v>100</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="N10" t="s">
@@ -1059,13 +1074,13 @@
       <c r="A11" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>53</v>
       </c>
       <c r="H11" t="s">
         <v>101</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="N11" t="s">
@@ -1076,7 +1091,7 @@
       <c r="A12" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>54</v>
       </c>
       <c r="H12" t="s">
@@ -1086,7 +1101,7 @@
         <f>M17</f>
         <v>H14</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="M12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="N12" t="s">
@@ -1097,13 +1112,13 @@
       <c r="A13" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>55</v>
       </c>
       <c r="H13" t="s">
         <v>112</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="M13" s="4" t="s">
         <v>32</v>
       </c>
       <c r="N13" t="s">
@@ -1118,13 +1133,13 @@
       <c r="A14" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>56</v>
       </c>
       <c r="H14" t="s">
         <v>113</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="4" t="s">
         <v>33</v>
       </c>
       <c r="N14" t="s">
@@ -1135,7 +1150,7 @@
       <c r="A15" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H15" t="s">
@@ -1147,7 +1162,7 @@
       <c r="J15" t="s">
         <v>117</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="4" t="s">
         <v>34</v>
       </c>
       <c r="N15" t="s">
@@ -1158,10 +1173,10 @@
       <c r="A16" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="M16" s="4" t="s">
         <v>35</v>
       </c>
       <c r="N16" t="s">
@@ -1172,10 +1187,10 @@
       <c r="A17" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="4" t="s">
         <v>36</v>
       </c>
       <c r="N17" t="s">
@@ -1186,10 +1201,10 @@
       <c r="A18" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="M18" s="4" t="s">
         <v>37</v>
       </c>
       <c r="N18" t="s">
@@ -1204,10 +1219,10 @@
       <c r="A19" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="M19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="N19" t="s">
@@ -1218,10 +1233,10 @@
       <c r="A20" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="M20" s="5" t="s">
+      <c r="M20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="N20" t="s">
@@ -1232,10 +1247,10 @@
       <c r="A21" t="s">
         <v>86</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M21" s="5" t="s">
+      <c r="M21" s="4" t="s">
         <v>40</v>
       </c>
       <c r="N21" t="s">
@@ -1246,10 +1261,10 @@
       <c r="A22" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="N22" t="s">
@@ -1263,10 +1278,10 @@
       <c r="A23" t="s">
         <v>88</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="M23" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1274,10 +1289,10 @@
       <c r="A24" t="s">
         <v>89</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="M24" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1285,10 +1300,10 @@
       <c r="A25" t="s">
         <v>90</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M25" s="5" t="s">
+      <c r="M25" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1296,10 +1311,10 @@
       <c r="A26" t="s">
         <v>91</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="M26" s="4" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added H3, updated H4 & H5, smaller improvements
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54267CD5-4741-4C17-818A-ABB8E58BC1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602C7A10-35EC-4C0C-87F4-33C85DD2DA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="127">
   <si>
     <t>Quests</t>
   </si>
@@ -405,13 +405,16 @@
     <t>%DoneSat</t>
   </si>
   <si>
-    <t>(silent creepy noise, footsteps, combination with light?)</t>
-  </si>
-  <si>
     <t>fusebox accessable</t>
   </si>
   <si>
-    <t>(MainSound(On/Off), FuseSound, metallic Box Sound, torchlight?)</t>
+    <t>(torchlight?)</t>
+  </si>
+  <si>
+    <t>(combination with light?)</t>
+  </si>
+  <si>
+    <t>((Message), look at window inpcmode)</t>
   </si>
 </sst>
 </file>
@@ -771,7 +774,7 @@
   <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="N5" sqref="N4:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,11 +903,17 @@
         <f>M7</f>
         <v>H4</v>
       </c>
+      <c r="K4" s="5">
+        <v>0.2</v>
+      </c>
       <c r="M4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="N4" t="s">
         <v>2</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>97</v>
@@ -941,6 +950,9 @@
       <c r="P5" t="s">
         <v>6</v>
       </c>
+      <c r="Q5" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -968,6 +980,12 @@
       <c r="P6" t="s">
         <v>12</v>
       </c>
+      <c r="Q6" s="5">
+        <v>0.93</v>
+      </c>
+      <c r="R6" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -989,13 +1007,13 @@
         <v>8</v>
       </c>
       <c r="P7" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0.97</v>
+      </c>
+      <c r="R7" t="s">
         <v>124</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>0.85</v>
-      </c>
-      <c r="R7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1019,10 +1037,10 @@
         <v>13</v>
       </c>
       <c r="Q8" s="5">
-        <v>0.85</v>
+        <v>0.97</v>
       </c>
       <c r="R8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1048,6 +1066,9 @@
       <c r="P9" t="s">
         <v>23</v>
       </c>
+      <c r="Q9" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1069,6 +1090,9 @@
         <f>M9</f>
         <v>H6</v>
       </c>
+      <c r="Q10" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1086,6 +1110,9 @@
       <c r="N11" t="s">
         <v>29</v>
       </c>
+      <c r="Q11" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1107,6 +1134,9 @@
       <c r="N12" t="s">
         <v>104</v>
       </c>
+      <c r="Q12" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1128,6 +1158,9 @@
         <f>G6</f>
         <v>T3</v>
       </c>
+      <c r="Q13" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1145,6 +1178,9 @@
       <c r="N14" t="s">
         <v>106</v>
       </c>
+      <c r="Q14" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1168,6 +1204,9 @@
       <c r="N15" t="s">
         <v>107</v>
       </c>
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1182,8 +1221,11 @@
       <c r="N16" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1196,8 +1238,11 @@
       <c r="N17" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1214,8 +1259,11 @@
         <f>G12</f>
         <v>T9</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -1228,8 +1276,11 @@
       <c r="N19" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -1242,8 +1293,11 @@
       <c r="N20" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -1256,8 +1310,11 @@
       <c r="N21" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -1273,8 +1330,11 @@
       <c r="P22" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1285,7 +1345,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -1296,7 +1356,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -1307,7 +1367,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -1325,7 +1385,7 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="Q1:Q1048576 V1:V1048576 K1:K1048576 E1:E1048576">
+  <conditionalFormatting sqref="V1:V1048576 K1:K1048576 E1:E1048576 Q1:Q1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
added H1; added flashlight for H4 (+ timer for the phone); smaller bug fixes
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602C7A10-35EC-4C0C-87F4-33C85DD2DA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621F448B-456A-4A81-8F48-F0D57A93A7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>RL Tasks</t>
   </si>
   <si>
-    <t>Phone rings</t>
-  </si>
-  <si>
     <t>Horror-Element</t>
   </si>
   <si>
@@ -414,7 +411,10 @@
     <t>(combination with light?)</t>
   </si>
   <si>
-    <t>((Message), look at window inpcmode)</t>
+    <t>((Message); look at window inpcmode; call police after reading message, but only a creepy tts answers ("1 1 0  1 1 0. We are here to… help help help. Affirmative. Target still alive", repeat sections, glitch effects))</t>
+  </si>
+  <si>
+    <t>Phone rings (multiple times)</t>
   </si>
 </sst>
 </file>
@@ -774,7 +774,7 @@
   <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N4:N5"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,88 +816,88 @@
       <c r="J2" s="7"/>
       <c r="K2" s="2"/>
       <c r="M2" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="2"/>
       <c r="S2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V2" s="2"/>
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="P3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="U3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" t="str">
         <f>M7</f>
@@ -907,164 +907,167 @@
         <v>0.2</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N4" t="s">
-        <v>2</v>
+        <v>126</v>
       </c>
       <c r="Q4" s="5">
         <v>0</v>
       </c>
       <c r="S4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="T4" t="s">
         <v>97</v>
       </c>
-      <c r="T4" t="s">
-        <v>98</v>
-      </c>
       <c r="U4" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
         <v>5</v>
       </c>
-      <c r="P5" t="s">
-        <v>6</v>
-      </c>
       <c r="Q5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" t="str">
         <f>CONCATENATE(G5,", ",S4)</f>
         <v>T2, O1</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q6" s="5">
-        <v>0.93</v>
+        <v>0.86</v>
       </c>
       <c r="R6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P7" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
         <v>123</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="R7" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I8" t="str">
         <f>G7</f>
         <v>T4</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q8" s="5">
         <v>0.97</v>
       </c>
       <c r="R8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" t="str">
         <f>G8</f>
         <v>T5</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q9" s="5">
         <v>0</v>
@@ -1072,19 +1075,19 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" t="s">
         <v>21</v>
-      </c>
-      <c r="N10" t="s">
-        <v>22</v>
       </c>
       <c r="O10" t="str">
         <f>M9</f>
@@ -1096,19 +1099,19 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q11" s="5">
         <v>0</v>
@@ -1116,23 +1119,23 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I12" t="str">
         <f>M17</f>
         <v>H14</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q12" s="5">
         <v>0</v>
@@ -1140,19 +1143,19 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O13" t="str">
         <f>G6</f>
@@ -1164,19 +1167,19 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q14" s="5">
         <v>0</v>
@@ -1184,25 +1187,25 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q15" s="5">
         <v>0</v>
@@ -1210,16 +1213,16 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q16" s="5">
         <v>0</v>
@@ -1227,16 +1230,16 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q17" s="5">
         <v>0</v>
@@ -1244,16 +1247,16 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O18" t="str">
         <f>G12</f>
@@ -1265,16 +1268,16 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q19" s="5">
         <v>0</v>
@@ -1282,16 +1285,16 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q20" s="5">
         <v>0</v>
@@ -1299,16 +1302,16 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q21" s="5">
         <v>0</v>
@@ -1316,19 +1319,19 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N22" t="s">
+        <v>118</v>
+      </c>
+      <c r="P22" t="s">
         <v>119</v>
-      </c>
-      <c r="P22" t="s">
-        <v>120</v>
       </c>
       <c r="Q22" s="5">
         <v>0</v>
@@ -1336,46 +1339,46 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added base for H13, fixed a sound bug, tiny other improvements
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5F1810-B467-49EF-82F1-C6EA1126BC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC61EF0B-691A-4E22-A04F-0810E4193BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>H7</t>
   </si>
   <si>
-    <t>Big spider crawls away after sight</t>
-  </si>
-  <si>
     <t>small spiders here and there?</t>
   </si>
   <si>
@@ -354,18 +351,12 @@
     <t>in game music gets creepy</t>
   </si>
   <si>
-    <t>in game spider jumps directly to the camera</t>
-  </si>
-  <si>
     <t>microwave suddenly starts</t>
   </si>
   <si>
     <t>stop microwave</t>
   </si>
   <si>
-    <t>innards in microwave for a short moments</t>
-  </si>
-  <si>
     <t>empty trash cans; bring trash to entrance door</t>
   </si>
   <si>
@@ -421,6 +412,15 @@
   </si>
   <si>
     <t>Big Spider jumps through gamePlayers face into metaPlayers face</t>
+  </si>
+  <si>
+    <t>innards in microwave for a short moment</t>
+  </si>
+  <si>
+    <t>Big spider(s) crawls away after sight</t>
+  </si>
+  <si>
+    <t>lower immersedvalue before so you aren't too close to the screen, fine tuning, reaction, crawling away</t>
   </si>
 </sst>
 </file>
@@ -780,7 +780,7 @@
   <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +829,7 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="2"/>
       <c r="S2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V2" s="2"/>
     </row>
@@ -847,7 +847,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
@@ -862,7 +862,7 @@
         <v>3</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>8</v>
@@ -877,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>8</v>
@@ -886,24 +886,24 @@
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" t="str">
         <f>M7</f>
@@ -916,19 +916,19 @@
         <v>14</v>
       </c>
       <c r="N4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Q4" s="5">
         <v>0</v>
       </c>
       <c r="S4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="T4" t="s">
         <v>95</v>
       </c>
-      <c r="T4" t="s">
-        <v>96</v>
-      </c>
       <c r="U4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V4" s="5">
         <v>0.5</v>
@@ -936,19 +936,19 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>15</v>
@@ -965,16 +965,16 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I6" t="str">
         <f>CONCATENATE(G5,", ",S4)</f>
@@ -993,21 +993,21 @@
         <v>0.86</v>
       </c>
       <c r="R6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>17</v>
@@ -1016,24 +1016,24 @@
         <v>7</v>
       </c>
       <c r="P7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="Q7" s="5">
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" t="str">
         <f>G7</f>
@@ -1049,18 +1049,18 @@
         <v>0.97</v>
       </c>
       <c r="R8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" t="str">
         <f>G8</f>
@@ -1073,7 +1073,7 @@
         <v>13</v>
       </c>
       <c r="P9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q9" s="5">
         <v>0</v>
@@ -1081,19 +1081,19 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="N10" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="O10" t="str">
         <f>M9</f>
@@ -1105,22 +1105,22 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q11" s="5">
         <v>1</v>
@@ -1128,23 +1128,23 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I12" t="str">
         <f>M17</f>
         <v>H14</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q12" s="5">
         <v>0</v>
@@ -1152,19 +1152,19 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O13" t="str">
         <f>G6</f>
@@ -1176,19 +1176,19 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q14" s="5">
         <v>1</v>
@@ -1196,25 +1196,25 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q15" s="5">
         <v>0</v>
@@ -1222,39 +1222,42 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N16" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="Q16" s="5">
-        <v>0</v>
+        <v>0.7</v>
+      </c>
+      <c r="R16" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q17" s="5">
         <v>0</v>
@@ -1262,16 +1265,16 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N18" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="O18" t="str">
         <f>G12</f>
@@ -1283,16 +1286,16 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Q19" s="5">
         <v>0</v>
@@ -1300,16 +1303,16 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q20" s="5">
         <v>0</v>
@@ -1317,16 +1320,16 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Q21" s="5">
         <v>0</v>
@@ -1334,19 +1337,19 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="Q22" s="5">
         <v>0</v>
@@ -1354,49 +1357,47 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N23" t="s">
-        <v>128</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="Q23" s="5"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added H19, H20; fixed small player unsneak bug
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B93206C-7754-4482-B730-101525A5E154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DC266E-1AEF-4FF0-B013-DBAF7883FD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,9 +381,6 @@
     <t>Light turns off randomly</t>
   </si>
   <si>
-    <t>randomly: glowing eyes in the room, disappearing when turning on the lights again</t>
-  </si>
-  <si>
     <t>Details</t>
   </si>
   <si>
@@ -424,6 +421,9 @@
   </si>
   <si>
     <t>crawling sfx?; spawn small spiders here and there (batches of ultra low poly spiders, slight movement with shaders maybe)</t>
+  </si>
+  <si>
+    <t>glowing eyes in a dark room, disappearing when turning on the lights</t>
   </si>
 </sst>
 </file>
@@ -783,7 +783,7 @@
   <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22:P22"/>
+      <selection activeCell="N20" sqref="N20:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +850,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
@@ -865,7 +865,7 @@
         <v>3</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>8</v>
@@ -880,7 +880,7 @@
         <v>3</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>8</v>
@@ -889,10 +889,10 @@
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -919,7 +919,7 @@
         <v>14</v>
       </c>
       <c r="N4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q4" s="5">
         <v>0</v>
@@ -977,7 +977,7 @@
         <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I6" t="str">
         <f>CONCATENATE(G5,", ",S4)</f>
@@ -996,7 +996,7 @@
         <v>0.86</v>
       </c>
       <c r="R6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1019,13 +1019,13 @@
         <v>7</v>
       </c>
       <c r="P7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q7" s="5">
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1052,7 +1052,7 @@
         <v>0.97</v>
       </c>
       <c r="R8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1082,7 +1082,7 @@
         <v>0.8</v>
       </c>
       <c r="R9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1099,7 +1099,7 @@
         <v>20</v>
       </c>
       <c r="N10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O10" t="str">
         <f>M9</f>
@@ -1234,7 +1234,7 @@
         <v>55</v>
       </c>
       <c r="H16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I16" t="s">
         <v>45</v>
@@ -1243,13 +1243,13 @@
         <v>32</v>
       </c>
       <c r="N16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q16" s="5">
         <v>0.7</v>
       </c>
       <c r="R16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1280,7 +1280,7 @@
         <v>34</v>
       </c>
       <c r="N18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O18" t="str">
         <f>G12</f>
@@ -1338,7 +1338,7 @@
         <v>111</v>
       </c>
       <c r="Q21" s="5">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -1354,11 +1354,8 @@
       <c r="N22" t="s">
         <v>114</v>
       </c>
-      <c r="P22" t="s">
-        <v>115</v>
-      </c>
       <c r="Q22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1371,7 +1368,12 @@
       <c r="M23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="Q23" s="5"/>
+      <c r="N23" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">

</xml_diff>

<commit_message>
added H17, small improvements to H6, H18, H19 and doors and lights in general
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DC266E-1AEF-4FF0-B013-DBAF7883FD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608C086F-4AA6-411F-ADEF-EE9BB8AE5C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -783,7 +783,7 @@
   <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20:N21"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,7 +1321,7 @@
         <v>110</v>
       </c>
       <c r="Q20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -1338,7 +1338,7 @@
         <v>111</v>
       </c>
       <c r="Q21" s="5">
-        <v>0.8</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added H14 (incl. microwave); swapped models for fridge, oven
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608C086F-4AA6-411F-ADEF-EE9BB8AE5C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CD3337-91C8-4010-AC48-339318633E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="131">
   <si>
     <t>Quests</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>glowing eyes in a dark room, disappearing when turning on the lights</t>
+  </si>
+  <si>
+    <t>add some harmless stuff in it</t>
   </si>
 </sst>
 </file>
@@ -783,7 +786,7 @@
   <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1255,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1266,10 +1269,13 @@
         <v>105</v>
       </c>
       <c r="Q17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+      <c r="R17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -1290,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -1307,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -1341,7 +1347,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1375,7 +1381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -1386,7 +1392,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
added H7; fixed door prefab; added H12
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CD3337-91C8-4010-AC48-339318633E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCA9908-CC17-4768-8153-2444699B8D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -786,7 +786,7 @@
   <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1052,7 @@
         <v>12</v>
       </c>
       <c r="Q8" s="5">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="R8" t="s">
         <v>119</v>
@@ -1109,7 +1109,7 @@
         <v>H6</v>
       </c>
       <c r="Q10" s="5">
-        <v>0</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1226,7 +1226,7 @@
         <v>104</v>
       </c>
       <c r="Q15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added H10, H15; (added food package)
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCA9908-CC17-4768-8153-2444699B8D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E49FB22-EFBC-4AC4-91D4-017B58AB822A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="133">
   <si>
     <t>Quests</t>
   </si>
@@ -342,9 +342,6 @@
     <t>basement door closes, traps you in; sth (glitchy monster/low poly monster without skin/goblin) slowly approaches player; door opens in the last second</t>
   </si>
   <si>
-    <t>food gets replaced with innards</t>
-  </si>
-  <si>
     <t>glass falls to the ground, breaks</t>
   </si>
   <si>
@@ -427,13 +424,22 @@
   </si>
   <si>
     <t>add some harmless stuff in it</t>
+  </si>
+  <si>
+    <t>pizza gets replaced with innards</t>
+  </si>
+  <si>
+    <t>flesh sounds, camera glitch effect? Or some other (glitchy?) effect when triggered</t>
+  </si>
+  <si>
+    <t>see H10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,13 +461,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -482,10 +500,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -494,6 +513,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -504,7 +524,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -786,7 +807,7 @@
   <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,26 +834,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="2"/>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
       <c r="K2" s="2"/>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
       <c r="Q2" s="2"/>
       <c r="S2" s="3" t="s">
         <v>93</v>
@@ -853,7 +874,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
@@ -868,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>8</v>
@@ -883,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>8</v>
@@ -892,10 +913,10 @@
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -922,7 +943,7 @@
         <v>14</v>
       </c>
       <c r="N4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q4" s="5">
         <v>0</v>
@@ -980,7 +1001,7 @@
         <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I6" t="str">
         <f>CONCATENATE(G5,", ",S4)</f>
@@ -999,7 +1020,7 @@
         <v>0.86</v>
       </c>
       <c r="R6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1022,13 +1043,13 @@
         <v>7</v>
       </c>
       <c r="P7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q7" s="5">
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1055,7 +1076,7 @@
         <v>0.95</v>
       </c>
       <c r="R8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1085,7 +1106,7 @@
         <v>0.8</v>
       </c>
       <c r="R9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1102,9 +1123,9 @@
         <v>20</v>
       </c>
       <c r="N10" t="s">
-        <v>126</v>
-      </c>
-      <c r="O10" t="str">
+        <v>125</v>
+      </c>
+      <c r="O10" s="6" t="str">
         <f>M9</f>
         <v>H6</v>
       </c>
@@ -1128,7 +1149,7 @@
       <c r="N11" t="s">
         <v>26</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="6" t="s">
         <v>55</v>
       </c>
       <c r="Q11" s="5">
@@ -1143,7 +1164,7 @@
         <v>51</v>
       </c>
       <c r="H12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I12" t="str">
         <f>M17</f>
@@ -1167,20 +1188,23 @@
         <v>52</v>
       </c>
       <c r="H13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="N13" t="s">
-        <v>102</v>
-      </c>
-      <c r="O13" t="str">
+        <v>130</v>
+      </c>
+      <c r="O13" s="6" t="str">
         <f>G6</f>
         <v>T3</v>
       </c>
       <c r="Q13" s="5">
-        <v>0</v>
+        <v>0.85</v>
+      </c>
+      <c r="R13" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1191,13 +1215,13 @@
         <v>53</v>
       </c>
       <c r="H14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="N14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q14" s="5">
         <v>1</v>
@@ -1211,19 +1235,19 @@
         <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I15" t="s">
         <v>28</v>
       </c>
       <c r="J15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>31</v>
       </c>
       <c r="N15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q15" s="5">
         <v>1</v>
@@ -1237,7 +1261,7 @@
         <v>55</v>
       </c>
       <c r="H16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I16" t="s">
         <v>45</v>
@@ -1246,13 +1270,13 @@
         <v>32</v>
       </c>
       <c r="N16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q16" s="5">
         <v>0.7</v>
       </c>
       <c r="R16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -1266,13 +1290,13 @@
         <v>33</v>
       </c>
       <c r="N17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q17" s="5">
         <v>0.8</v>
       </c>
       <c r="R17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1286,14 +1310,17 @@
         <v>34</v>
       </c>
       <c r="N18" t="s">
-        <v>125</v>
-      </c>
-      <c r="O18" t="str">
+        <v>124</v>
+      </c>
+      <c r="O18" s="6" t="str">
         <f>G12</f>
         <v>T9</v>
       </c>
       <c r="Q18" s="5">
-        <v>0</v>
+        <v>0.99</v>
+      </c>
+      <c r="R18" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -1307,7 +1334,7 @@
         <v>35</v>
       </c>
       <c r="N19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q19" s="5">
         <v>0</v>
@@ -1324,7 +1351,7 @@
         <v>36</v>
       </c>
       <c r="N20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q20" s="5">
         <v>1</v>
@@ -1341,7 +1368,7 @@
         <v>37</v>
       </c>
       <c r="N21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q21" s="5">
         <v>0.99</v>
@@ -1358,7 +1385,7 @@
         <v>38</v>
       </c>
       <c r="N22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q22" s="5">
         <v>1</v>
@@ -1375,7 +1402,7 @@
         <v>39</v>
       </c>
       <c r="N23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q23" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
added H1; fixed/improved H4; small refractoring
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E49FB22-EFBC-4AC4-91D4-017B58AB822A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560E2171-AF40-446D-85FA-B96F520545E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="134">
   <si>
     <t>Quests</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>see H10</t>
+  </si>
+  <si>
+    <t>more calls, 3d audio?</t>
   </si>
 </sst>
 </file>
@@ -807,7 +810,7 @@
   <dimension ref="A2:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N19" sqref="N19:Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +949,10 @@
         <v>120</v>
       </c>
       <c r="Q4" s="5">
-        <v>0</v>
+        <v>0.98</v>
+      </c>
+      <c r="R4" t="s">
+        <v>133</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
added quest animations with sound effect
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B090EFD2-6306-49AF-84ED-5235D9C00A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E962BC7-20AA-4080-ADB5-586E656E4948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,7 +445,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +470,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -506,11 +513,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -529,8 +537,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -812,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +836,7 @@
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -846,7 +860,7 @@
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="10"/>
       <c r="G2" s="7" t="s">
         <v>1</v>
       </c>
@@ -879,7 +893,7 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="11" t="s">
         <v>114</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -932,6 +946,9 @@
       <c r="B4" t="s">
         <v>89</v>
       </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
       <c r="G4" s="4" t="s">
         <v>43</v>
       </c>
@@ -977,6 +994,9 @@
       <c r="B5" t="s">
         <v>90</v>
       </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
       <c r="G5" s="4" t="s">
         <v>44</v>
       </c>
@@ -1006,6 +1026,9 @@
       <c r="B6" t="s">
         <v>91</v>
       </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
       <c r="G6" s="4" t="s">
         <v>45</v>
       </c>
@@ -1038,6 +1061,9 @@
       </c>
       <c r="B7" t="s">
         <v>92</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
adjusted dialogue; improved freezing of players; added first version of rl-tasks-manager
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E962BC7-20AA-4080-ADB5-586E656E4948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D78D41A-A088-43AD-B5A0-4B3F94467060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="136">
   <si>
     <t>Quests</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>put pizza(/fries/cheese-sticks) in oven (one at a time, if it burns -&gt; next one; if nothing is left -&gt; monster waits in the freezer, kills you)</t>
+  </si>
+  <si>
+    <t>Order</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -528,6 +531,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -537,11 +545,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Prozent" xfId="2" builtinId="5"/>
@@ -824,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:V26"/>
+  <dimension ref="A2:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,51 +842,53 @@
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-      <c r="G2" s="7" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="7"/>
+      <c r="G2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="2"/>
-      <c r="M2" s="7" t="s">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="2"/>
+      <c r="N2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="2"/>
-      <c r="S2" s="3" t="s">
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="2"/>
+      <c r="T2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="V2" s="2"/>
-    </row>
-    <row r="3" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W2" s="2"/>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -893,601 +901,643 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="8" t="s">
         <v>114</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="14">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="str">
-        <f>M7</f>
+      <c r="J4" t="str">
+        <f>N7</f>
         <v>H4</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <v>0.6</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>119</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="R4" s="5">
         <v>0.98</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>132</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>95</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>98</v>
       </c>
-      <c r="V4" s="5">
+      <c r="W4" s="5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="14">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
         <v>134</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>99</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>4</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>5</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="R5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
       <c r="B6" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="14">
+        <v>32</v>
+      </c>
+      <c r="I6" t="s">
         <v>121</v>
       </c>
-      <c r="I6" t="str">
-        <f>CONCATENATE(G5,", ",S4)</f>
+      <c r="J6" t="str">
+        <f>CONCATENATE(G5,", ",T4)</f>
         <v>T2, O1</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>6</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>11</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="R6" s="5">
         <v>0.86</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
       <c r="B7" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="14">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="N7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>7</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>115</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="R7" s="5">
         <v>1</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="15">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
         <v>24</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" t="str">
         <f>G7</f>
         <v>T4</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="R8" s="5">
         <v>0.95</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="15">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
         <v>25</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" t="str">
         <f>G8</f>
         <v>T5</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>13</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="R9" s="5">
         <v>0.8</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="15">
+        <v>41</v>
+      </c>
+      <c r="I10" t="s">
         <v>96</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="N10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>124</v>
       </c>
-      <c r="O10" s="6" t="str">
-        <f>M9</f>
+      <c r="P10" s="6" t="str">
+        <f>N9</f>
         <v>H6</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="R10" s="5">
         <v>0.99</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>73</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="15">
+        <v>42</v>
+      </c>
+      <c r="I11" t="s">
         <v>97</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="P11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="R11" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>74</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="15">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
         <v>104</v>
       </c>
-      <c r="I12" t="str">
-        <f>M17</f>
+      <c r="J12" t="str">
+        <f>N17</f>
         <v>H14</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>100</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="R12" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="15">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
         <v>105</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>129</v>
       </c>
-      <c r="O13" s="6" t="str">
+      <c r="P13" s="6" t="str">
         <f>G6</f>
         <v>T3</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="R13" s="5">
         <v>0.85</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="15">
+        <v>22</v>
+      </c>
+      <c r="I14" t="s">
         <v>106</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="N14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>101</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="R14" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="14">
+        <v>52</v>
+      </c>
+      <c r="I15" t="s">
         <v>111</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>28</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>110</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>102</v>
       </c>
-      <c r="Q15" s="5">
+      <c r="R15" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>78</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="14">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
         <v>120</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="N16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>122</v>
       </c>
-      <c r="Q16" s="5">
+      <c r="R16" s="5">
         <v>0.7</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="N17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>103</v>
       </c>
-      <c r="Q17" s="5">
+      <c r="R17" s="5">
         <v>0.8</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="N18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>123</v>
       </c>
-      <c r="O18" s="6" t="str">
+      <c r="P18" s="6" t="str">
         <f>G12</f>
         <v>T9</v>
       </c>
-      <c r="Q18" s="5">
+      <c r="R18" s="5">
         <v>0.99</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="N19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>107</v>
       </c>
-      <c r="Q19" s="5">
+      <c r="R19" s="5">
         <v>0.9</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="N20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>108</v>
       </c>
-      <c r="Q20" s="5">
+      <c r="R20" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>83</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="N21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>109</v>
       </c>
-      <c r="Q21" s="5">
+      <c r="R21" s="5">
         <v>0.99</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="N22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>112</v>
       </c>
-      <c r="Q22" s="5">
+      <c r="R22" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="N23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>127</v>
       </c>
-      <c r="Q23" s="5">
+      <c r="R23" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>86</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M24" s="4" t="s">
+      <c r="N24" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>87</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="M25" s="4" t="s">
+      <c r="N25" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>88</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="N26" s="4" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="G2:K2"/>
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="V1:V1048576 K1:K1048576 E1:E1048576 Q1:Q1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="W1:W1048576 L1:L1048576 E1:E1048576 R1:R1048576">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1496,7 +1546,40 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D71621EC-D14F-4285-BBB7-4E999731B8FB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D71621EC-D14F-4285-BBB7-4E999731B8FB}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H1:H1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added intro cutscene ("fake trailer")
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D78D41A-A088-43AD-B5A0-4B3F94467060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FA36CA-C302-4486-B83D-AE2DA4DED698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="139">
   <si>
     <t>Quests</t>
   </si>
@@ -336,9 +336,6 @@
     <t>starts O1, shows timer on phone</t>
   </si>
   <si>
-    <t>basement door closes, traps you in; sth (glitchy monster/low poly monster without skin/goblin) slowly approaches player; door opens in the last second</t>
-  </si>
-  <si>
     <t>glass falls to the ground, breaks</t>
   </si>
   <si>
@@ -442,6 +439,18 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>basement door closes, traps you in; sth (glitchy monster/low poly monster without skin) slowly approaches player; door opens in the last second</t>
+  </si>
+  <si>
+    <t>Glitchy Monster appears in-game (cave?), walks slowly to player, teleports if necessary, touches player -&gt; small chirp+glitchy screep for a second, then everything is normal again and the monster is gone</t>
+  </si>
+  <si>
+    <t>What to do better</t>
+  </si>
+  <si>
+    <t>End: You die somehow (maybe: door leads to inGame, you get drowned by a slime)</t>
   </si>
 </sst>
 </file>
@@ -536,6 +545,9 @@
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -545,9 +557,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Prozent" xfId="2" builtinId="5"/>
@@ -832,9 +841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -844,7 +851,7 @@
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="31.7109375" bestFit="1" customWidth="1"/>
@@ -861,27 +868,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="2"/>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
       <c r="R2" s="2"/>
       <c r="T2" s="3" t="s">
         <v>93</v>
@@ -902,13 +909,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>135</v>
+      <c r="H3" s="10" t="s">
+        <v>134</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>9</v>
@@ -920,7 +927,7 @@
         <v>3</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>8</v>
@@ -935,7 +942,10 @@
         <v>3</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>8</v>
@@ -944,10 +954,10 @@
         <v>9</v>
       </c>
       <c r="V3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -963,7 +973,7 @@
       <c r="G4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="11">
         <v>43</v>
       </c>
       <c r="I4" t="s">
@@ -980,13 +990,13 @@
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R4" s="5">
         <v>0.98</v>
       </c>
       <c r="S4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T4" s="4" t="s">
         <v>94</v>
@@ -1014,11 +1024,11 @@
       <c r="G5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="11">
         <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K5" t="s">
         <v>99</v>
@@ -1049,11 +1059,11 @@
       <c r="G6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="11">
         <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J6" t="str">
         <f>CONCATENATE(G5,", ",T4)</f>
@@ -1072,7 +1082,7 @@
         <v>0.86</v>
       </c>
       <c r="S6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -1088,7 +1098,7 @@
       <c r="G7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="11">
         <v>11</v>
       </c>
       <c r="I7" t="s">
@@ -1101,13 +1111,13 @@
         <v>7</v>
       </c>
       <c r="Q7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R7" s="5">
         <v>1</v>
       </c>
       <c r="S7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -1117,7 +1127,7 @@
       <c r="G8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="12">
         <v>12</v>
       </c>
       <c r="I8" t="s">
@@ -1137,7 +1147,7 @@
         <v>0.95</v>
       </c>
       <c r="S8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -1147,7 +1157,7 @@
       <c r="G9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="12">
         <v>13</v>
       </c>
       <c r="I9" t="s">
@@ -1170,7 +1180,7 @@
         <v>0.8</v>
       </c>
       <c r="S9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -1180,7 +1190,7 @@
       <c r="G10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="12">
         <v>41</v>
       </c>
       <c r="I10" t="s">
@@ -1190,7 +1200,7 @@
         <v>20</v>
       </c>
       <c r="O10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P10" s="6" t="str">
         <f>N9</f>
@@ -1207,11 +1217,14 @@
       <c r="G11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="12">
         <v>42</v>
       </c>
       <c r="I11" t="s">
         <v>97</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>27</v>
@@ -1233,11 +1246,11 @@
       <c r="G12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="12">
         <v>51</v>
       </c>
       <c r="I12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J12" t="str">
         <f>N17</f>
@@ -1247,7 +1260,10 @@
         <v>28</v>
       </c>
       <c r="O12" t="s">
-        <v>100</v>
+        <v>135</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="R12" s="5">
         <v>0</v>
@@ -1260,17 +1276,17 @@
       <c r="G13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="12">
         <v>21</v>
       </c>
       <c r="I13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P13" s="6" t="str">
         <f>G6</f>
@@ -1280,7 +1296,7 @@
         <v>0.85</v>
       </c>
       <c r="S13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1290,17 +1306,17 @@
       <c r="G14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="12">
         <v>22</v>
       </c>
       <c r="I14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="O14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R14" s="5">
         <v>1</v>
@@ -1313,23 +1329,23 @@
       <c r="G15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="11">
         <v>52</v>
       </c>
       <c r="I15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J15" t="s">
         <v>28</v>
       </c>
       <c r="K15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R15" s="5">
         <v>1</v>
@@ -1342,11 +1358,11 @@
       <c r="G16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="11">
         <v>33</v>
       </c>
       <c r="I16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J16" t="s">
         <v>45</v>
@@ -1355,13 +1371,13 @@
         <v>32</v>
       </c>
       <c r="O16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R16" s="5">
         <v>0.7</v>
       </c>
       <c r="S16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -1375,13 +1391,13 @@
         <v>33</v>
       </c>
       <c r="O17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R17" s="5">
         <v>0.8</v>
       </c>
       <c r="S17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1395,7 +1411,7 @@
         <v>34</v>
       </c>
       <c r="O18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P18" s="6" t="str">
         <f>G12</f>
@@ -1405,7 +1421,7 @@
         <v>0.99</v>
       </c>
       <c r="S18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -1419,13 +1435,13 @@
         <v>35</v>
       </c>
       <c r="O19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R19" s="5">
         <v>0.9</v>
       </c>
       <c r="S19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1439,7 +1455,7 @@
         <v>36</v>
       </c>
       <c r="O20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R20" s="5">
         <v>1</v>
@@ -1456,7 +1472,7 @@
         <v>37</v>
       </c>
       <c r="O21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R21" s="5">
         <v>0.99</v>
@@ -1473,7 +1489,7 @@
         <v>38</v>
       </c>
       <c r="O22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R22" s="5">
         <v>1</v>
@@ -1490,7 +1506,7 @@
         <v>39</v>
       </c>
       <c r="O23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R23" s="5">
         <v>1</v>
@@ -1506,6 +1522,12 @@
       <c r="N24" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="O24" t="s">
+        <v>136</v>
+      </c>
+      <c r="R24" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1516,6 +1538,12 @@
       </c>
       <c r="N25" s="4" t="s">
         <v>41</v>
+      </c>
+      <c r="O25" t="s">
+        <v>138</v>
+      </c>
+      <c r="R25" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added brightness slider; improved some things; added Tasks T4, T5, T6
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FA36CA-C302-4486-B83D-AE2DA4DED698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37EBE4B-84BB-4761-B571-7259C4102326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="141">
   <si>
     <t>Quests</t>
   </si>
@@ -451,6 +451,12 @@
   </si>
   <si>
     <t>End: You die somehow (maybe: door leads to inGame, you get drowned by a slime)</t>
+  </si>
+  <si>
+    <t>connections, dialogue</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -841,7 +847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -929,6 +937,9 @@
       <c r="L3" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="M3" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="N3" s="3" t="s">
         <v>8</v>
       </c>
@@ -986,6 +997,9 @@
       <c r="L4" s="5">
         <v>0.6</v>
       </c>
+      <c r="M4" t="s">
+        <v>139</v>
+      </c>
       <c r="N4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1104,6 +1118,12 @@
       <c r="I7" t="s">
         <v>23</v>
       </c>
+      <c r="L7" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="M7" t="s">
+        <v>140</v>
+      </c>
       <c r="N7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1137,6 +1157,9 @@
         <f>G7</f>
         <v>T4</v>
       </c>
+      <c r="L8" s="5">
+        <v>0.9</v>
+      </c>
       <c r="N8" s="4" t="s">
         <v>18</v>
       </c>
@@ -1166,6 +1189,9 @@
       <c r="J9" t="str">
         <f>G8</f>
         <v>T5</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0.9</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>19</v>
@@ -1564,7 +1590,7 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="W1:W1048576 L1:L1048576 E1:E1048576 R1:R1048576">
+  <conditionalFormatting sqref="W1:W1048576 E1:E1048576 R1:R1048576 L1:L1048576">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
added tasks T10, T11
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37EBE4B-84BB-4761-B571-7259C4102326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989D1E46-0B2F-40AF-B936-0D8D4D034889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="141">
   <si>
     <t>Quests</t>
   </si>
@@ -456,7 +456,7 @@
     <t>connections, dialogue</t>
   </si>
   <si>
-    <t>time</t>
+    <t>more sfx</t>
   </si>
 </sst>
 </file>
@@ -565,9 +565,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
-    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -848,10 +848,10 @@
   <dimension ref="A2:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -1308,6 +1308,12 @@
       <c r="I13" t="s">
         <v>104</v>
       </c>
+      <c r="L13" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="M13" t="s">
+        <v>140</v>
+      </c>
       <c r="N13" s="4" t="s">
         <v>29</v>
       </c>
@@ -1337,6 +1343,9 @@
       </c>
       <c r="I14" t="s">
         <v>105</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0.9</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
added T2[, T3] (biggest/main task)
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989D1E46-0B2F-40AF-B936-0D8D4D034889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFEB19E-67DD-4011-8CCB-E2C26DF33D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="143">
   <si>
     <t>Quests</t>
   </si>
@@ -456,14 +456,20 @@
     <t>connections, dialogue</t>
   </si>
   <si>
-    <t>more sfx</t>
+    <t>more sfx, more animations</t>
+  </si>
+  <si>
+    <t>more sfx, outside, more animations</t>
+  </si>
+  <si>
+    <t>sound effects, models, details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,6 +499,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -536,7 +550,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,6 +577,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -848,7 +864,7 @@
   <dimension ref="A2:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,13 +1028,13 @@
       <c r="S4" t="s">
         <v>131</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="T4" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="16" t="s">
         <v>98</v>
       </c>
       <c r="W4" s="5">
@@ -1047,10 +1063,16 @@
       <c r="K5" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="L5" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="M5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="Q5" t="s">
@@ -1070,7 +1092,7 @@
       <c r="E6" s="9">
         <v>1</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="17" t="s">
         <v>45</v>
       </c>
       <c r="H6" s="11">
@@ -1083,6 +1105,9 @@
         <f>CONCATENATE(G5,", ",T4)</f>
         <v>T2, O1</v>
       </c>
+      <c r="L6" s="5">
+        <v>0.85</v>
+      </c>
       <c r="N6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1119,7 +1144,7 @@
         <v>23</v>
       </c>
       <c r="L7" s="5">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="M7" t="s">
         <v>140</v>
@@ -1158,7 +1183,7 @@
         <v>T4</v>
       </c>
       <c r="L8" s="5">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>18</v>
@@ -1191,7 +1216,7 @@
         <v>T5</v>
       </c>
       <c r="L9" s="5">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>19</v>
@@ -1222,6 +1247,9 @@
       <c r="I10" t="s">
         <v>96</v>
       </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
       <c r="N10" s="4" t="s">
         <v>20</v>
       </c>
@@ -1252,6 +1280,12 @@
       <c r="J11" t="s">
         <v>40</v>
       </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
       <c r="N11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1282,6 +1316,9 @@
         <f>N17</f>
         <v>H14</v>
       </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
       <c r="N12" s="4" t="s">
         <v>28</v>
       </c>
@@ -1312,7 +1349,7 @@
         <v>0.9</v>
       </c>
       <c r="M13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>29</v>
@@ -1376,6 +1413,9 @@
       <c r="K15" t="s">
         <v>109</v>
       </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
       <c r="N15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1401,6 +1441,9 @@
       </c>
       <c r="J16" t="s">
         <v>45</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
extended H8, H10; added T13
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFEB19E-67DD-4011-8CCB-E2C26DF33D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD907BC-61DC-468F-A6EC-29AC08F855CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="145">
   <si>
     <t>Quests</t>
   </si>
@@ -420,12 +420,6 @@
     <t>add some harmless stuff in it</t>
   </si>
   <si>
-    <t>pizza gets replaced with innards</t>
-  </si>
-  <si>
-    <t>flesh sounds, camera glitch effect? Or some other (glitchy?) effect when triggered</t>
-  </si>
-  <si>
     <t>see H10</t>
   </si>
   <si>
@@ -463,6 +457,18 @@
   </si>
   <si>
     <t>sound effects, models, details</t>
+  </si>
+  <si>
+    <t>T3, H10</t>
+  </si>
+  <si>
+    <t>pizza gets replaced with innards, plate breaks</t>
+  </si>
+  <si>
+    <t>flesh sounds, plate sounds, camera glitch effect? Or some other (glitchy?) effect when triggered</t>
+  </si>
+  <si>
+    <t>sfx, better reason, say "no soap" when trying to use other sink</t>
   </si>
 </sst>
 </file>
@@ -568,6 +574,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -577,8 +585,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -864,7 +870,7 @@
   <dimension ref="A2:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I10" sqref="I10:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,27 +898,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="2"/>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
       <c r="R2" s="2"/>
       <c r="T2" s="3" t="s">
         <v>93</v>
@@ -939,7 +945,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>9</v>
@@ -954,7 +960,7 @@
         <v>113</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>8</v>
@@ -972,7 +978,7 @@
         <v>113</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>8</v>
@@ -1014,7 +1020,7 @@
         <v>0.6</v>
       </c>
       <c r="M4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>14</v>
@@ -1026,15 +1032,15 @@
         <v>0.98</v>
       </c>
       <c r="S4" t="s">
-        <v>131</v>
-      </c>
-      <c r="T4" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="T4" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="U4" s="16" t="s">
+      <c r="U4" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="V4" s="16" t="s">
+      <c r="V4" s="13" t="s">
         <v>98</v>
       </c>
       <c r="W4" s="5">
@@ -1058,7 +1064,7 @@
         <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K5" t="s">
         <v>99</v>
@@ -1067,12 +1073,12 @@
         <v>0.85</v>
       </c>
       <c r="M5" t="s">
-        <v>142</v>
-      </c>
-      <c r="N5" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="N5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="O5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="Q5" t="s">
@@ -1092,7 +1098,7 @@
       <c r="E6" s="9">
         <v>1</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="14" t="s">
         <v>45</v>
       </c>
       <c r="H6" s="11">
@@ -1147,7 +1153,7 @@
         <v>0.95</v>
       </c>
       <c r="M7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>17</v>
@@ -1323,7 +1329,7 @@
         <v>28</v>
       </c>
       <c r="O12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>50</v>
@@ -1349,13 +1355,13 @@
         <v>0.9</v>
       </c>
       <c r="M13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O13" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="P13" s="6" t="str">
         <f>G6</f>
@@ -1365,7 +1371,7 @@
         <v>0.85</v>
       </c>
       <c r="S13" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1440,10 +1446,13 @@
         <v>119</v>
       </c>
       <c r="J16" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="L16" s="5">
-        <v>0</v>
+        <v>0.9</v>
+      </c>
+      <c r="M16" t="s">
+        <v>144</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>32</v>
@@ -1499,7 +1508,7 @@
         <v>0.99</v>
       </c>
       <c r="S18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -1519,7 +1528,7 @@
         <v>0.9</v>
       </c>
       <c r="S19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1601,7 +1610,7 @@
         <v>40</v>
       </c>
       <c r="O24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R24" s="5">
         <v>0</v>
@@ -1618,7 +1627,7 @@
         <v>41</v>
       </c>
       <c r="O25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R25" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
connected all tasks, quests and horror events
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F6F5F7-24B4-4256-B935-00CEBB81C447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FB804A-3FA2-4AA4-92C3-B5702837A77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="179">
   <si>
     <t>Quests</t>
   </si>
@@ -342,9 +342,6 @@
     <t>microwave suddenly starts</t>
   </si>
   <si>
-    <t>stop microwave</t>
-  </si>
-  <si>
     <t>empty trash cans; bring trash to entrance door</t>
   </si>
   <si>
@@ -417,9 +414,6 @@
     <t>see H10</t>
   </si>
   <si>
-    <t>more calls, 3d audio?</t>
-  </si>
-  <si>
     <t>sfx?, better DestroyWhenNotLooking?</t>
   </si>
   <si>
@@ -453,9 +447,6 @@
     <t>sound effects, models, details</t>
   </si>
   <si>
-    <t>T3, H10</t>
-  </si>
-  <si>
     <t>pizza gets replaced with innards, plate breaks</t>
   </si>
   <si>
@@ -484,13 +475,109 @@
   </si>
   <si>
     <t>sfx, camera effects (both stronger when near it), prevent player from squesszing past it, details, more dialogue?</t>
+  </si>
+  <si>
+    <t>When</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Decoration(water bottle, more glasses)</t>
+  </si>
+  <si>
+    <t>x sec after H9</t>
+  </si>
+  <si>
+    <t>shortly after T3</t>
+  </si>
+  <si>
+    <t>during T13</t>
+  </si>
+  <si>
+    <t>once for each location after H6</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>with T9</t>
+  </si>
+  <si>
+    <t>In Q4 after entering the cave</t>
+  </si>
+  <si>
+    <t>starts H22</t>
+  </si>
+  <si>
+    <t>after T8</t>
+  </si>
+  <si>
+    <t>after Q4 after exiting the cave</t>
+  </si>
+  <si>
+    <t>after T1 after going upstairs</t>
+  </si>
+  <si>
+    <t>after T12</t>
+  </si>
+  <si>
+    <t>(x sec after intro)</t>
+  </si>
+  <si>
+    <t>(T4 etc.)</t>
+  </si>
+  <si>
+    <t>(^)</t>
+  </si>
+  <si>
+    <t>after T8 after sitting down after x sec</t>
+  </si>
+  <si>
+    <t>(after T2, x sec after Q3, x sec after sitting down)</t>
+  </si>
+  <si>
+    <t>T2, O1</t>
+  </si>
+  <si>
+    <t>during T11</t>
+  </si>
+  <si>
+    <t>(after T6, x sec after Q2, x sec after sitting down)</t>
+  </si>
+  <si>
+    <t>dialogue, call ends automatically, more calls, 3d audio?</t>
+  </si>
+  <si>
+    <t>during T12 after entering the basement</t>
+  </si>
+  <si>
+    <t>after T8, after going upstairs</t>
+  </si>
+  <si>
+    <t>once at the beginning of T4</t>
+  </si>
+  <si>
+    <t>(optional) stop microwave</t>
+  </si>
+  <si>
+    <t>(With H14)</t>
+  </si>
+  <si>
+    <t>(H14)</t>
+  </si>
+  <si>
+    <t>after T4, during T2, during T12</t>
+  </si>
+  <si>
+    <t>during T14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,13 +601,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -534,8 +614,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,11 +638,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -565,13 +664,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -580,17 +695,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -600,11 +720,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -882,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:W26"/>
+  <dimension ref="A2:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,9 +1016,9 @@
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="31.7109375" bestFit="1" customWidth="1"/>
@@ -905,42 +1027,45 @@
     <col min="15" max="15" width="46.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.7109375" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.7109375" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="7"/>
-      <c r="G2" s="15" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="6"/>
+      <c r="G2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
       <c r="L2" s="2"/>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="2"/>
-      <c r="T2" s="3" t="s">
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="2"/>
+      <c r="U2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="W2" s="2"/>
-    </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -953,14 +1078,14 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>112</v>
+      <c r="E3" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>130</v>
+      <c r="H3" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>9</v>
@@ -972,10 +1097,10 @@
         <v>3</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>8</v>
@@ -990,96 +1115,104 @@
         <v>3</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="T3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="11">
-        <v>43</v>
+      <c r="H4" s="10">
+        <v>47</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" t="str">
-        <f>N7</f>
-        <v>H4</v>
+      <c r="J4" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="L4" s="5">
         <v>0.6</v>
       </c>
       <c r="M4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>116</v>
-      </c>
-      <c r="R4" s="5">
-        <v>0.98</v>
-      </c>
-      <c r="S4" t="s">
-        <v>127</v>
-      </c>
-      <c r="T4" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="R4" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="T4" t="s">
+        <v>170</v>
+      </c>
+      <c r="U4" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="U4" s="13" t="s">
+      <c r="V4" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="V4" s="13" t="s">
+      <c r="W4" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="W4" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>169</v>
       </c>
       <c r="K5" t="s">
         <v>98</v>
@@ -1088,43 +1221,45 @@
         <v>0.85</v>
       </c>
       <c r="M5" t="s">
-        <v>138</v>
-      </c>
-      <c r="N5" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="N5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="Q5" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="S5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
       <c r="B6" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>1</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>118</v>
-      </c>
-      <c r="J6" t="str">
-        <f>CONCATENATE(G5,", ",T4)</f>
-        <v>T2, O1</v>
+        <v>117</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>167</v>
       </c>
       <c r="L6" s="5">
         <v>0.85</v>
@@ -1138,37 +1273,43 @@
       <c r="Q6" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="S6" s="5">
         <v>0.86</v>
       </c>
-      <c r="S6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
       <c r="B7" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>11</v>
       </c>
       <c r="I7" t="s">
         <v>23</v>
       </c>
+      <c r="J7" s="16" t="s">
+        <v>162</v>
+      </c>
       <c r="L7" s="5">
         <v>0.95</v>
       </c>
       <c r="M7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>17</v>
@@ -1177,31 +1318,33 @@
         <v>7</v>
       </c>
       <c r="Q7" t="s">
-        <v>144</v>
-      </c>
-      <c r="R7" s="5">
+        <v>141</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="S7" s="5">
         <v>1</v>
       </c>
-      <c r="S7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <v>12</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
       </c>
-      <c r="J8" t="str">
-        <f>G7</f>
-        <v>T4</v>
+      <c r="J8" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="L8" s="5">
         <v>0.95</v>
@@ -1212,29 +1355,31 @@
       <c r="O8" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="S8" s="5">
         <v>0.95</v>
       </c>
-      <c r="S8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <v>13</v>
       </c>
       <c r="I9" t="s">
         <v>25</v>
       </c>
-      <c r="J9" t="str">
-        <f>G8</f>
-        <v>T5</v>
+      <c r="J9" s="16" t="s">
+        <v>47</v>
       </c>
       <c r="L9" s="5">
         <v>0.95</v>
@@ -1248,25 +1393,31 @@
       <c r="Q9" t="s">
         <v>21</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="S9" s="5">
         <v>0.8</v>
       </c>
-      <c r="S9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="11">
         <v>41</v>
       </c>
       <c r="I10" t="s">
-        <v>143</v>
+        <v>140</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="L10" s="5">
         <v>0.99</v>
@@ -1275,31 +1426,34 @@
         <v>20</v>
       </c>
       <c r="O10" t="s">
-        <v>121</v>
-      </c>
-      <c r="P10" s="6" t="str">
+        <v>120</v>
+      </c>
+      <c r="P10" t="str">
         <f>N9</f>
         <v>H6</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="S10" s="5">
         <v>0.99</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>73</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="11">
         <v>42</v>
       </c>
       <c r="I11" t="s">
         <v>96</v>
       </c>
-      <c r="J11" t="s">
-        <v>40</v>
+      <c r="J11" s="16" t="s">
+        <v>164</v>
       </c>
       <c r="K11" t="s">
         <v>28</v>
@@ -1313,100 +1467,117 @@
       <c r="O11" t="s">
         <v>26</v>
       </c>
-      <c r="P11" s="6" t="s">
+      <c r="P11" t="s">
         <v>55</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="S11" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>74</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <v>51</v>
       </c>
       <c r="I12" t="s">
-        <v>102</v>
-      </c>
-      <c r="J12" t="str">
-        <f>N17</f>
-        <v>H14</v>
+        <v>174</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>176</v>
       </c>
       <c r="L12" s="5">
         <v>0.6</v>
       </c>
       <c r="M12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>28</v>
       </c>
       <c r="O12" t="s">
-        <v>131</v>
-      </c>
-      <c r="P12" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="P12" t="s">
         <v>50</v>
       </c>
-      <c r="R12" s="5">
+      <c r="Q12" t="s">
+        <v>157</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="S12" s="5">
         <v>0.8</v>
       </c>
-      <c r="S12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="11">
         <v>21</v>
       </c>
       <c r="I13" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="L13" s="5">
         <v>0.9</v>
       </c>
       <c r="M13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O13" t="s">
-        <v>140</v>
-      </c>
-      <c r="P13" s="6" t="str">
+        <v>137</v>
+      </c>
+      <c r="P13" t="str">
         <f>G6</f>
         <v>T3</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="S13" s="5">
         <v>0.85</v>
       </c>
-      <c r="S13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="11">
         <v>22</v>
       </c>
       <c r="I14" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>164</v>
       </c>
       <c r="L14" s="5">
         <v>0.9</v>
@@ -1417,34 +1588,40 @@
       <c r="O14" t="s">
         <v>99</v>
       </c>
-      <c r="R14" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R14" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="T14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <v>52</v>
       </c>
       <c r="I15" t="s">
-        <v>109</v>
-      </c>
-      <c r="J15" t="s">
-        <v>28</v>
+        <v>108</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>175</v>
       </c>
       <c r="K15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L15" s="5">
         <v>0.85</v>
       </c>
       <c r="M15" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>31</v>
@@ -1452,69 +1629,75 @@
       <c r="O15" t="s">
         <v>100</v>
       </c>
-      <c r="R15" s="5">
+      <c r="R15" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="S15" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>78</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <v>33</v>
       </c>
       <c r="I16" t="s">
-        <v>117</v>
-      </c>
-      <c r="J16" t="s">
-        <v>139</v>
+        <v>116</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="L16" s="5">
         <v>0.9</v>
       </c>
       <c r="M16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>32</v>
       </c>
       <c r="O16" t="s">
-        <v>119</v>
-      </c>
-      <c r="R16" s="5">
+        <v>118</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="S16" s="5">
         <v>0.7</v>
       </c>
-      <c r="S16" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="11">
         <v>61</v>
       </c>
       <c r="I17" t="s">
-        <v>146</v>
-      </c>
-      <c r="J17" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" s="16" t="s">
         <v>54</v>
       </c>
       <c r="K17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L17" s="5">
         <v>0.9</v>
       </c>
       <c r="M17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>33</v>
@@ -1522,14 +1705,17 @@
       <c r="O17" t="s">
         <v>101</v>
       </c>
-      <c r="R17" s="5">
+      <c r="R17" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="S17" s="5">
         <v>0.8</v>
       </c>
-      <c r="S17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -1540,20 +1726,23 @@
         <v>34</v>
       </c>
       <c r="O18" t="s">
-        <v>120</v>
-      </c>
-      <c r="P18" s="6" t="str">
+        <v>119</v>
+      </c>
+      <c r="P18" t="str">
         <f>G12</f>
         <v>T9</v>
       </c>
-      <c r="R18" s="5">
+      <c r="R18" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="S18" s="5">
         <v>0.99</v>
       </c>
-      <c r="S18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -1564,16 +1753,19 @@
         <v>35</v>
       </c>
       <c r="O19" t="s">
-        <v>105</v>
-      </c>
-      <c r="R19" s="5">
+        <v>104</v>
+      </c>
+      <c r="R19" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="S19" s="5">
         <v>0.9</v>
       </c>
-      <c r="S19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -1584,13 +1776,16 @@
         <v>36</v>
       </c>
       <c r="O20" t="s">
-        <v>106</v>
-      </c>
-      <c r="R20" s="5">
+        <v>105</v>
+      </c>
+      <c r="R20" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="S20" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -1601,13 +1796,16 @@
         <v>37</v>
       </c>
       <c r="O21" t="s">
-        <v>107</v>
-      </c>
-      <c r="R21" s="5">
+        <v>106</v>
+      </c>
+      <c r="R21" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="S21" s="5">
         <v>0.99</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1618,13 +1816,16 @@
         <v>38</v>
       </c>
       <c r="O22" t="s">
-        <v>110</v>
-      </c>
-      <c r="R22" s="5">
+        <v>109</v>
+      </c>
+      <c r="R22" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="S22" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1635,13 +1836,16 @@
         <v>39</v>
       </c>
       <c r="O23" t="s">
-        <v>124</v>
-      </c>
-      <c r="R23" s="5">
+        <v>123</v>
+      </c>
+      <c r="R23" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="S23" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -1652,13 +1856,16 @@
         <v>40</v>
       </c>
       <c r="O24" t="s">
-        <v>132</v>
-      </c>
-      <c r="R24" s="5">
+        <v>130</v>
+      </c>
+      <c r="R24" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="S24" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -1669,13 +1876,16 @@
         <v>41</v>
       </c>
       <c r="O25" t="s">
-        <v>134</v>
-      </c>
-      <c r="R25" s="5">
+        <v>132</v>
+      </c>
+      <c r="R25" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="S25" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -1693,7 +1903,7 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="W1:W1048576 E1:E1048576 R1:R1048576 L1:L1048576">
+  <conditionalFormatting sqref="X1:X1048576 E1:E1048576 L1:L1048576 R1:S1048576">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
updated unity; added promo stuff; fixed small game breaking bug
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FB804A-3FA2-4AA4-92C3-B5702837A77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A89D1FB-E8D9-4865-9CA9-488155D4EF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -711,6 +711,7 @@
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="9" fontId="6" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -720,7 +721,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,27 +1037,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="6"/>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="2"/>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
       <c r="R2" s="14"/>
       <c r="S2" s="2"/>
       <c r="U2" s="3" t="s">
@@ -1170,7 +1170,7 @@
       <c r="O4" t="s">
         <v>115</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="18" t="s">
         <v>177</v>
       </c>
       <c r="S4" s="5">
@@ -1273,7 +1273,7 @@
       <c r="Q6" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="21" t="s">
+      <c r="R6" s="18" t="s">
         <v>172</v>
       </c>
       <c r="S6" s="5">
@@ -1629,7 +1629,7 @@
       <c r="O15" t="s">
         <v>100</v>
       </c>
-      <c r="R15" s="21" t="s">
+      <c r="R15" s="18" t="s">
         <v>158</v>
       </c>
       <c r="S15" s="5">
@@ -1881,8 +1881,8 @@
       <c r="R25" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="S25" s="17">
-        <v>0</v>
+      <c r="S25" s="5">
+        <v>0.9</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reworked quest system; updated unity; removed some .blend1 files
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BC983B-D7D3-443D-8D8E-1FFA1CE84342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27676AAE-F53A-4AE3-9D93-F21C730C505F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="166">
   <si>
     <t>Quests</t>
   </si>
@@ -297,9 +297,6 @@
     <t>Q22</t>
   </si>
   <si>
-    <t>Q23</t>
-  </si>
-  <si>
     <t>Speak with the king</t>
   </si>
   <si>
@@ -312,21 +309,9 @@
     <t>kill the cave boss</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>O1</t>
-  </si>
-  <si>
-    <t>Pizza-Timer</t>
-  </si>
-  <si>
     <t>get crackers from the basement</t>
   </si>
   <si>
-    <t>pizza is done after 10 "minutes", is burned after 2 more "minutes"</t>
-  </si>
-  <si>
     <t>starts O1, shows timer on phone</t>
   </si>
   <si>
@@ -363,12 +348,6 @@
     <t>Light turns off randomly</t>
   </si>
   <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>%DoneSat</t>
-  </si>
-  <si>
     <t>Phone rings (multiple times)</t>
   </si>
   <si>
@@ -513,16 +492,46 @@
     <t>small spiders here and there</t>
   </si>
   <si>
-    <t>reach level 20</t>
-  </si>
-  <si>
-    <t>kill 5 spiders</t>
-  </si>
-  <si>
-    <t>buy another staff and armor</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> duel with fake player to death</t>
+    <t>Kill 5 Spiders and 5 Rats</t>
+  </si>
+  <si>
+    <t>reach currentLevel+10</t>
+  </si>
+  <si>
+    <t>buy 2nd Tier staff and armor</t>
+  </si>
+  <si>
+    <t>Find out if there are goblins in the cave</t>
+  </si>
+  <si>
+    <t>Reach Level 2M</t>
+  </si>
+  <si>
+    <t>Find a repairman for fixing the cart blocking the bridge</t>
+  </si>
+  <si>
+    <t>Find out what exactly is blocking the bridge</t>
+  </si>
+  <si>
+    <t>Duel with a fake player that talks too much</t>
+  </si>
+  <si>
+    <t>Report back to the king that a goblin was sighted at the cave</t>
+  </si>
+  <si>
+    <t>cave boss spawns now</t>
+  </si>
+  <si>
+    <t>Find the ultimate spell (a scroll) -&gt; spell is an "epic" spell that kills everything (player too)</t>
+  </si>
+  <si>
+    <t>one goblin spawns</t>
+  </si>
+  <si>
+    <t>all goblins spawn now (except the boss)</t>
+  </si>
+  <si>
+    <t>QEnd</t>
   </si>
 </sst>
 </file>
@@ -954,15 +963,15 @@
   <dimension ref="A2:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.28515625" bestFit="1" customWidth="1"/>
@@ -1000,9 +1009,7 @@
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
       <c r="N2" s="18"/>
-      <c r="O2" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="O2" s="3"/>
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1013,7 +1020,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
@@ -1022,7 +1029,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -1046,27 +1053,19 @@
         <v>3</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>110</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>42</v>
@@ -1084,30 +1083,25 @@
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="R4" s="5">
-        <v>1</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="5"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>43</v>
@@ -1116,13 +1110,13 @@
         <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="I5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>15</v>
@@ -1134,7 +1128,7 @@
         <v>5</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1142,7 +1136,10 @@
         <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>44</v>
@@ -1151,10 +1148,10 @@
         <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>16</v>
@@ -1166,7 +1163,7 @@
         <v>11</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1174,7 +1171,13 @@
         <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>161</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>45</v>
@@ -1186,7 +1189,7 @@
         <v>22</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>17</v>
@@ -1195,10 +1198,10 @@
         <v>7</v>
       </c>
       <c r="M7" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1206,7 +1209,13 @@
         <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>153</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>164</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>46</v>
@@ -1227,7 +1236,7 @@
         <v>12</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1235,7 +1244,10 @@
         <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>152</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>47</v>
@@ -1256,10 +1268,10 @@
         <v>13</v>
       </c>
       <c r="M9" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1267,7 +1279,10 @@
         <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>48</v>
@@ -1276,23 +1291,23 @@
         <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="K10" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="L10" t="str">
         <f>J9</f>
         <v>H6</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1300,7 +1315,10 @@
         <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>157</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>49</v>
@@ -1309,10 +1327,10 @@
         <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="I11" t="s">
         <v>27</v>
@@ -1327,13 +1345,19 @@
         <v>54</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
+      <c r="B12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
       <c r="E12" s="4" t="s">
         <v>50</v>
       </c>
@@ -1341,31 +1365,40 @@
         <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>27</v>
       </c>
       <c r="K12" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="L12" t="s">
         <v>49</v>
       </c>
       <c r="M12" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>74</v>
       </c>
+      <c r="B13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>163</v>
+      </c>
       <c r="E13" s="4" t="s">
         <v>51</v>
       </c>
@@ -1373,29 +1406,35 @@
         <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="K13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="L13" t="str">
         <f>E6</f>
         <v>T3</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>75</v>
       </c>
+      <c r="B14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
       <c r="E14" s="4" t="s">
         <v>52</v>
       </c>
@@ -1403,25 +1442,31 @@
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="N14" s="11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>76</v>
       </c>
+      <c r="B15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15">
+        <v>21</v>
+      </c>
       <c r="E15" s="4" t="s">
         <v>53</v>
       </c>
@@ -1429,28 +1474,34 @@
         <v>52</v>
       </c>
       <c r="G15" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="I15" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="N15" s="14" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>77</v>
       </c>
+      <c r="B16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16">
+        <v>22</v>
+      </c>
       <c r="E16" s="4" t="s">
         <v>54</v>
       </c>
@@ -1458,7 +1509,7 @@
         <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>28</v>
@@ -1467,10 +1518,10 @@
         <v>31</v>
       </c>
       <c r="K16" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="N16" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1484,22 +1535,22 @@
         <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>53</v>
       </c>
       <c r="I17" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K17" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N17" s="11" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1513,14 +1564,14 @@
         <v>33</v>
       </c>
       <c r="K18" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="L18" t="str">
         <f>E12</f>
         <v>T9</v>
       </c>
       <c r="N18" s="11" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1534,10 +1585,10 @@
         <v>34</v>
       </c>
       <c r="K19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="N19" s="11" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1551,10 +1602,10 @@
         <v>35</v>
       </c>
       <c r="K20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N20" s="11" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1568,10 +1619,10 @@
         <v>36</v>
       </c>
       <c r="K21" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1585,10 +1636,10 @@
         <v>37</v>
       </c>
       <c r="K22" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="N22" s="11" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1602,10 +1653,10 @@
         <v>38</v>
       </c>
       <c r="K23" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="N23" s="11" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1619,10 +1670,10 @@
         <v>39</v>
       </c>
       <c r="K24" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -1636,15 +1687,21 @@
         <v>40</v>
       </c>
       <c r="K25" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>165</v>
+      </c>
+      <c r="B26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26">
+        <v>23</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>64</v>
@@ -1661,7 +1718,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="R1:R1048576 N1 N3:N1048576">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1684,6 +1741,20 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C1048576 C1:C16">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C277B040-2905-41DC-AC5B-C44743FBF08E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
@@ -1691,16 +1762,25 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D71621EC-D14F-4285-BBB7-4E999731B8FB}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>F1:F1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C277B040-2905-41DC-AC5B-C44743FBF08E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C22:C1048576 C1:C16</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
added new horror event (H23)
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27676AAE-F53A-4AE3-9D93-F21C730C505F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E53178-96F8-4333-8990-C89AA3277F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="168">
   <si>
     <t>Quests</t>
   </si>
@@ -532,13 +532,19 @@
   </si>
   <si>
     <t>QEnd</t>
+  </si>
+  <si>
+    <t>spawning after Q8</t>
+  </si>
+  <si>
+    <t>Goblin in real environment and car in game environment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,40 +574,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -619,21 +601,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -643,12 +610,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -662,10 +627,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,13 +636,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Gut" xfId="1" builtinId="26"/>
-    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -963,7 +922,7 @@
   <dimension ref="A2:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,26 +948,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="15" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="18"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="14"/>
       <c r="O2" s="3"/>
       <c r="R2" s="2"/>
     </row>
@@ -1076,7 +1035,7 @@
       <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -1085,7 +1044,7 @@
       <c r="K4" t="s">
         <v>104</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" t="s">
         <v>149</v>
       </c>
       <c r="O4" s="10"/>
@@ -1112,7 +1071,7 @@
       <c r="G5" t="s">
         <v>111</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" t="s">
         <v>142</v>
       </c>
       <c r="I5" t="s">
@@ -1127,7 +1086,7 @@
       <c r="M5" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1150,7 +1109,7 @@
       <c r="G6" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" t="s">
         <v>140</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -1162,7 +1121,7 @@
       <c r="M6" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1188,7 +1147,7 @@
       <c r="G7" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" t="s">
         <v>135</v>
       </c>
       <c r="J7" s="4" t="s">
@@ -1200,7 +1159,7 @@
       <c r="M7" t="s">
         <v>118</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1226,7 +1185,7 @@
       <c r="G8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" t="s">
         <v>45</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1235,7 +1194,7 @@
       <c r="K8" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="N8" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1258,7 +1217,7 @@
       <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" t="s">
         <v>46</v>
       </c>
       <c r="J9" s="4" t="s">
@@ -1270,7 +1229,7 @@
       <c r="M9" t="s">
         <v>151</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="N9" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1293,7 +1252,7 @@
       <c r="G10" t="s">
         <v>117</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" t="s">
         <v>139</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -1306,7 +1265,7 @@
         <f>J9</f>
         <v>H6</v>
       </c>
-      <c r="N10" s="13" t="s">
+      <c r="N10" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1329,7 +1288,7 @@
       <c r="G11" t="s">
         <v>91</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" t="s">
         <v>137</v>
       </c>
       <c r="I11" t="s">
@@ -1344,7 +1303,7 @@
       <c r="L11" t="s">
         <v>54</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="N11" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1367,7 +1326,7 @@
       <c r="G12" t="s">
         <v>146</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" t="s">
         <v>148</v>
       </c>
       <c r="J12" s="4" t="s">
@@ -1382,7 +1341,7 @@
       <c r="M12" t="s">
         <v>130</v>
       </c>
-      <c r="N12" s="11" t="s">
+      <c r="N12" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1408,7 +1367,7 @@
       <c r="G13" t="s">
         <v>96</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" t="s">
         <v>136</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1421,7 +1380,7 @@
         <f>E6</f>
         <v>T3</v>
       </c>
-      <c r="N13" s="11" t="s">
+      <c r="N13" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1444,7 +1403,7 @@
       <c r="G14" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" t="s">
         <v>137</v>
       </c>
       <c r="J14" s="4" t="s">
@@ -1453,7 +1412,7 @@
       <c r="K14" t="s">
         <v>93</v>
       </c>
-      <c r="N14" s="11" t="s">
+      <c r="N14" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1476,7 +1435,7 @@
       <c r="G15" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" t="s">
         <v>147</v>
       </c>
       <c r="I15" t="s">
@@ -1488,7 +1447,7 @@
       <c r="K15" t="s">
         <v>94</v>
       </c>
-      <c r="N15" s="14" t="s">
+      <c r="N15" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1511,7 +1470,7 @@
       <c r="G16" t="s">
         <v>105</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" t="s">
         <v>28</v>
       </c>
       <c r="J16" s="4" t="s">
@@ -1520,7 +1479,7 @@
       <c r="K16" t="s">
         <v>107</v>
       </c>
-      <c r="N16" s="11" t="s">
+      <c r="N16" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1537,7 +1496,7 @@
       <c r="G17" t="s">
         <v>120</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" t="s">
         <v>53</v>
       </c>
       <c r="I17" t="s">
@@ -1549,7 +1508,7 @@
       <c r="K17" t="s">
         <v>95</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="N17" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1570,7 +1529,7 @@
         <f>E12</f>
         <v>T9</v>
       </c>
-      <c r="N18" s="11" t="s">
+      <c r="N18" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1587,7 +1546,7 @@
       <c r="K19" t="s">
         <v>98</v>
       </c>
-      <c r="N19" s="11" t="s">
+      <c r="N19" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1604,7 +1563,7 @@
       <c r="K20" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="N20" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1621,7 +1580,7 @@
       <c r="K21" t="s">
         <v>100</v>
       </c>
-      <c r="N21" s="11" t="s">
+      <c r="N21" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1638,7 +1597,7 @@
       <c r="K22" t="s">
         <v>103</v>
       </c>
-      <c r="N22" s="11" t="s">
+      <c r="N22" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1655,7 +1614,7 @@
       <c r="K23" t="s">
         <v>110</v>
       </c>
-      <c r="N23" s="11" t="s">
+      <c r="N23" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1672,7 +1631,7 @@
       <c r="K24" t="s">
         <v>114</v>
       </c>
-      <c r="N24" s="13" t="s">
+      <c r="N24" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1689,7 +1648,7 @@
       <c r="K25" t="s">
         <v>115</v>
       </c>
-      <c r="N25" s="13" t="s">
+      <c r="N25" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1708,6 +1667,12 @@
       </c>
       <c r="J26" s="4" t="s">
         <v>41</v>
+      </c>
+      <c r="K26" t="s">
+        <v>167</v>
+      </c>
+      <c r="N26" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added H24 and more
</commit_message>
<xml_diff>
--- a/Documents/StoryElements.xlsx
+++ b/Documents/StoryElements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8B538E-6E78-4874-BC74-B4041AC8549B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628D530B-0A24-45B0-B756-C2769E7C0EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="171">
   <si>
     <t>Quests</t>
   </si>
@@ -538,6 +538,15 @@
   </si>
   <si>
     <t>Goblin in real environment and car in game environment</t>
+  </si>
+  <si>
+    <t>H24</t>
+  </si>
+  <si>
+    <t>Stalker at Backdoor/Entrance/Kitchen Window</t>
+  </si>
+  <si>
+    <t>Once per location, randomly after the middle of T2</t>
   </si>
 </sst>
 </file>
@@ -627,6 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -639,7 +649,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -920,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R26"/>
+  <dimension ref="A2:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,26 +958,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="11" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="11" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="14"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="15"/>
       <c r="O2" s="3"/>
       <c r="R2" s="2"/>
     </row>
@@ -1321,7 +1330,7 @@
       <c r="E12" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="11">
         <v>51</v>
       </c>
       <c r="G12" s="9" t="s">
@@ -1674,6 +1683,17 @@
       </c>
       <c r="N26" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J27" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="K27" t="s">
+        <v>169</v>
+      </c>
+      <c r="N27" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>